<commit_message>
unique validation, upload - download, session, scroll to top button
</commit_message>
<xml_diff>
--- a/public/Students.xlsx
+++ b/public/Students.xlsx
@@ -53,12 +53,6 @@
     <t>square@pan.ts</t>
   </si>
   <si>
-    <t>Najmuddin</t>
-  </si>
-  <si>
-    <t>najmuddin@mail.com</t>
-  </si>
-  <si>
     <t>Diana</t>
   </si>
   <si>
@@ -117,6 +111,12 @@
   </si>
   <si>
     <t>fsddsaf@fd.sd</t>
+  </si>
+  <si>
+    <t>gksjad</t>
+  </si>
+  <si>
+    <t>fsdck@mail.sd</t>
   </si>
 </sst>
 </file>
@@ -524,69 +524,69 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>12345669</v>
+        <v>12345467</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>12345467</v>
+        <v>87654321</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>87654321</v>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
         <v>20</v>
+      </c>
+      <c r="B8">
+        <v>76583421</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9">
-        <v>76583421</v>
+        <v>56742123</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -594,13 +594,13 @@
         <v>25</v>
       </c>
       <c r="B10">
-        <v>56742123</v>
+        <v>98765437</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -608,27 +608,27 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <v>98765437</v>
+        <v>76567875</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12">
-        <v>76567875</v>
+        <v>56137565</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -636,7 +636,7 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>56137565</v>
+        <v>87436252</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Insert Excel data to DB
</commit_message>
<xml_diff>
--- a/public/Students.xlsx
+++ b/public/Students.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,15 @@
     <t>Department</t>
   </si>
   <si>
+    <t>Bintang Diyantoro</t>
+  </si>
+  <si>
+    <t>bintangdiyantoro@gmail.com</t>
+  </si>
+  <si>
+    <t>Technique Informatique</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
@@ -42,9 +51,6 @@
   </si>
   <si>
     <t>be@n.com</t>
-  </si>
-  <si>
-    <t>Technique Informatique</t>
   </si>
   <si>
     <t>Sponge's Bob</t>
@@ -455,7 +461,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>89234238</v>
+        <v>12345678</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -496,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>12345679</v>
+        <v>89234238</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -510,13 +516,13 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>12345677</v>
+        <v>12345679</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -524,69 +530,69 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>12345467</v>
+        <v>12345677</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>12345467</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>87654321</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>87654321</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
-      </c>
-      <c r="B8">
-        <v>76583421</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>76583421</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
-        <v>56742123</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -594,13 +600,13 @@
         <v>25</v>
       </c>
       <c r="B10">
-        <v>98765437</v>
+        <v>56742123</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -608,27 +614,27 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <v>76567875</v>
+        <v>98765437</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>76567875</v>
+      </c>
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
-        <v>56137565</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -636,13 +642,27 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>87436252</v>
+        <v>56137565</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>87436252</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>